<commit_message>
Update the time schedule
</commit_message>
<xml_diff>
--- a/Process_Documents/Project timeline.xlsx
+++ b/Process_Documents/Project timeline.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985ED886-B30D-48FE-B944-44A313A2B864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Project Timeline'!$A$1:$L$14</definedName>
     <definedName name="ProjectEnd">INDEX(ProjectDetails[],MIN(ROW(data))+ROWS(data)-1,1)</definedName>
     <definedName name="ProjectStart">ProjectDetails[]('Project Timeline'!$B$17)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Project Timeline'!$A$1:$L$14</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Project Timeline</t>
   </si>
@@ -74,9 +75,6 @@
     <t>DRTS</t>
   </si>
   <si>
-    <t>MCP</t>
-  </si>
-  <si>
     <t>Model ready</t>
   </si>
   <si>
@@ -97,11 +95,29 @@
   <si>
     <t>SEMCON</t>
   </si>
+  <si>
+    <t>MVC</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Controller design - MPC</t>
+  </si>
+  <si>
+    <t>Controller design - LQR</t>
+  </si>
+  <si>
+    <t>Controller design - PI</t>
+  </si>
+  <si>
+    <t>Controller Test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
@@ -109,7 +125,7 @@
     <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
@@ -211,6 +227,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -237,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -260,6 +283,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -277,7 +311,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -377,6 +411,9 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -386,20 +423,41 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Comma" xfId="6" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="7" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="8" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="9" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Bemærk!" xfId="11" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Komma" xfId="6" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Komma [0]" xfId="7" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="11" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="10" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Procent" xfId="10" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Valuta" xfId="8" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Valuta [0]" xfId="9" builtinId="7" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -467,7 +525,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Project Timeline" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Project Timeline" pivot="0" count="2">
+    <tableStyle name="Project Timeline" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
     </tableStyle>
@@ -486,7 +544,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -553,7 +611,7 @@
                     <a:fld id="{38BBA013-30A3-4E6C-A1D3-5EF6D1513EB1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -561,9 +619,9 @@
                     <a:fld id="{695A9D1D-15EE-425F-A650-75662AB74DA2}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -578,7 +636,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -603,7 +660,7 @@
                     <a:fld id="{3AEDABC0-ED0B-4B29-B966-F0824DBF65DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -611,9 +668,9 @@
                     <a:fld id="{8ADBBBA2-1DBF-4F21-A72E-E068DE7E37C1}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -628,7 +685,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -653,7 +709,7 @@
                     <a:fld id="{89C66AAD-5390-4101-A161-865A928CC1AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -661,9 +717,9 @@
                     <a:fld id="{EFC92BFA-4E62-46E3-9E76-D1EBE8419B53}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -678,7 +734,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -703,7 +758,7 @@
                     <a:fld id="{EF4A7E30-7AF8-4233-B90F-4C5786D1B879}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -711,9 +766,9 @@
                     <a:fld id="{BA519C51-CDAD-4385-B9A0-6D3A04256C2F}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -728,7 +783,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -753,7 +807,7 @@
                     <a:fld id="{41AC6839-2D7B-4CE5-BC64-BDE049CAC51D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -761,9 +815,9 @@
                     <a:fld id="{37131ACD-84F4-42EB-814F-3CBCFA9F05AF}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -778,7 +832,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -803,7 +856,7 @@
                     <a:fld id="{CE72315B-35BD-4F85-A731-B5509EE2FDF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -811,9 +864,9 @@
                     <a:fld id="{A55CB0EC-89B2-467B-85A1-0549DB7653E7}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -828,7 +881,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -853,7 +905,7 @@
                     <a:fld id="{F1682120-E413-489F-BBFC-DA651141CB86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -861,9 +913,9 @@
                     <a:fld id="{DF5C3B40-E92F-4EB1-808D-51167C502D28}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -878,7 +930,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -903,7 +954,7 @@
                     <a:fld id="{9100B6D6-BCD7-4526-B0FA-27C34E1F9D33}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -911,9 +962,9 @@
                     <a:fld id="{63F6FEE7-E7B9-47A4-AD99-F858ED888535}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -928,7 +979,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -953,7 +1003,7 @@
                     <a:fld id="{3385B721-571E-4BBB-A385-E771BDC53DC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -961,9 +1011,9 @@
                     <a:fld id="{266135CB-479F-4905-A553-8B3EA861FA68}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -978,7 +1028,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1003,7 +1052,7 @@
                     <a:fld id="{70EBAD28-6B3E-4AD0-BE0D-03059317BF5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -1011,9 +1060,9 @@
                     <a:fld id="{E2100826-A16D-4679-AF10-D241A3D148C0}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1028,7 +1077,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1053,7 +1101,7 @@
                     <a:fld id="{AE0859E4-BF7E-44F5-AA70-6251FE00BDB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -1061,9 +1109,9 @@
                     <a:fld id="{0617D681-6427-422C-86DC-EE73622515E9}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1078,7 +1126,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1103,7 +1150,7 @@
                     <a:fld id="{85C1A84E-729C-4046-8960-A8CB5BD2C35F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -1111,9 +1158,9 @@
                     <a:fld id="{0D95E02C-930F-4864-9E58-3980F3EDDDF4}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1128,7 +1175,6 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1153,7 +1199,7 @@
                     <a:fld id="{6765A073-0BC3-43F1-944D-00DF9C4FC898}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
+                      <a:t>[CELLEOMRÅDE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -1161,9 +1207,9 @@
                     <a:fld id="{4DCF4CA1-F86D-4829-92FB-8AD8358ACA12}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CATEGORY NAME]</a:t>
+                      <a:t>[KATEGORINAVN]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="da-DK"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1183,6 +1229,190 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000C-B7D0-4032-AD18-593E91345D5E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{4CBB92B9-30E3-409E-BFC4-48CBCAEA1C1E}" type="CELLRANGE">
+                      <a:rPr lang="da-DK"/>
+                      <a:pPr/>
+                      <a:t>[CELLEOMRÅDE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="da-DK" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{590F4631-499D-4EBC-9160-3F27A5554F25}" type="CATEGORYNAME">
+                      <a:rPr lang="da-DK" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[KATEGORINAVN]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="da-DK" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-AEA5-4D5A-81F1-1F5A54365187}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{887817AB-3B35-49BD-A177-9FA1F424C2D6}" type="CELLRANGE">
+                      <a:rPr lang="da-DK"/>
+                      <a:pPr/>
+                      <a:t>[CELLEOMRÅDE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="da-DK" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{2B7F2235-1ED0-49B7-BF87-1895F0A875CC}" type="CATEGORYNAME">
+                      <a:rPr lang="da-DK" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[KATEGORINAVN]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="da-DK" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-AEA5-4D5A-81F1-1F5A54365187}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{945A5D8F-B858-433E-946B-5E0630C94E11}" type="CELLRANGE">
+                      <a:rPr lang="da-DK"/>
+                      <a:pPr/>
+                      <a:t>[CELLEOMRÅDE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="da-DK" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{11A36EAB-533A-46DC-BD68-BD66624AA5EA}" type="CATEGORYNAME">
+                      <a:rPr lang="da-DK" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[KATEGORINAVN]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="da-DK" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-AEA5-4D5A-81F1-1F5A54365187}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6F17526A-0153-4456-B75B-4ED7CE350ACB}" type="CELLRANGE">
+                      <a:rPr lang="da-DK"/>
+                      <a:pPr/>
+                      <a:t>[CELLEOMRÅDE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="da-DK" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{7051F969-B92F-4058-893F-C4812A504F62}" type="CATEGORYNAME">
+                      <a:rPr lang="da-DK" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[KATEGORINAVN]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="da-DK" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-AEA5-4D5A-81F1-1F5A54365187}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1207,7 +1437,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="da-DK"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1259,9 +1489,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Project Timeline'!$C$17:$C$28</c:f>
+              <c:f>'Project Timeline'!$C$17:$C$33</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>Project Start</c:v>
                 </c:pt>
@@ -1269,33 +1499,48 @@
                   <c:v>Model ready</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MCP</c:v>
+                  <c:v>MVC</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Simulation</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Measure in LAB</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>Controller design - PI</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Controller design - LQR</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>STOK</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
+                  <c:v>Controller design - MPC</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Controller Test</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Artikel+Abstract</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>DRTS</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>Review(s)</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>Project done</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>Project delivery</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
                   <c:v>SEMCON</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>Project End</c:v>
                 </c:pt>
               </c:strCache>
@@ -1303,10 +1548,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Project Timeline'!$E$17:$E$28</c:f>
+              <c:f>'Project Timeline'!$E$17:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1320,16 +1565,16 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>20</c:v>
@@ -1341,6 +1586,21 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -1349,9 +1609,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>'Project Timeline'!$D$17:$D$28</c15:f>
+                <c15:f>'Project Timeline'!$D$17:$D$33</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="12"/>
+                  <c:ptCount val="17"/>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -1445,44 +1705,59 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>'Project Timeline'!$B$17:$B$28</c:f>
+              <c:f>'Project Timeline'!$B$17:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>44470</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44481</c:v>
+                  <c:v>44489</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>44495</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>44496</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="m/d/yyyy">
                   <c:v>44501</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5" formatCode="m/d/yyyy">
+                  <c:v>44505</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="m/d/yyyy">
+                  <c:v>44512</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="m/d/yyyy">
                   <c:v>44516</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8" formatCode="m/d/yyyy">
+                  <c:v>44518</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="m/d/yyyy">
+                  <c:v>44525</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="m/d/yyyy">
                   <c:v>44526</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11" formatCode="m/d/yyyy">
                   <c:v>44529</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12" formatCode="m/d/yyyy">
                   <c:v>44538</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13" formatCode="m/d/yyyy">
                   <c:v>44545</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14" formatCode="m/d/yyyy">
                   <c:v>44547</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15" formatCode="m/d/yyyy">
                   <c:v>44551</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16" formatCode="m/d/yyyy">
                   <c:v>44562</c:v>
                 </c:pt>
               </c:numCache>
@@ -1490,10 +1765,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Project Timeline'!$F$17:$F$29</c:f>
+              <c:f>'Project Timeline'!$F$17:$F$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1531,6 +1806,21 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1592,7 +1882,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="717044496"/>
@@ -1685,7 +1975,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2184,16 +2474,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ProjectDetails" displayName="ProjectDetails" ref="B16:F29" totalsRowShown="0" headerRowDxfId="3">
-  <sortState ref="B17:F30">
-    <sortCondition ref="B21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ProjectDetails" displayName="ProjectDetails" ref="B16:F34" totalsRowShown="0" headerRowDxfId="3">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B17:F35">
+    <sortCondition ref="B26"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Date" dataDxfId="2"/>
-    <tableColumn id="2" name="Milestone" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="Assigned To" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Position" dataDxfId="0"/>
-    <tableColumn id="5" name="Baseline">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Milestone" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Assigned To" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Position" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Baseline">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2468,15 +2758,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2495,10 +2785,10 @@
   <sheetData>
     <row r="1" spans="1:12" s="24" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2510,175 +2800,175 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
     </row>
     <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
     </row>
     <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
     </row>
     <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
     </row>
     <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
     </row>
     <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
     </row>
     <row r="11" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
     </row>
     <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
     </row>
     <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
     </row>
     <row r="14" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
     </row>
     <row r="15" spans="1:12" s="26" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
@@ -2712,10 +3002,10 @@
       <c r="F16" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="34"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="3"/>
       <c r="L16" s="3"/>
     </row>
@@ -2734,20 +3024,20 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
     </row>
     <row r="18" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
-        <v>44481</v>
+        <v>44489</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18"/>
       <c r="E18" s="9">
@@ -2757,18 +3047,18 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
     </row>
     <row r="19" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13">
         <v>44495</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D19"/>
       <c r="E19" s="9">
@@ -2778,220 +3068,325 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
     </row>
     <row r="20" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="13">
-        <v>44501</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20"/>
-      <c r="E20" s="9">
+      <c r="B20" s="39">
+        <v>44496</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="41">
         <v>20</v>
       </c>
       <c r="F20" s="10">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
     </row>
     <row r="21" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="13">
-        <v>44516</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21"/>
-      <c r="E21" s="9">
-        <v>-10</v>
+      <c r="B21" s="42">
+        <v>44501</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="41">
+        <v>10</v>
       </c>
       <c r="F21" s="10">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
     </row>
     <row r="22" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="13">
-        <v>44526</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22"/>
-      <c r="E22" s="9">
+      <c r="B22" s="38">
+        <v>44505</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="43">
         <v>20</v>
       </c>
       <c r="F22" s="10">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
     </row>
     <row r="23" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="13">
-        <v>44529</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23"/>
-      <c r="E23" s="9">
-        <v>-10</v>
+      <c r="B23" s="38">
+        <v>44512</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="43">
+        <v>10</v>
       </c>
       <c r="F23" s="10">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
     </row>
     <row r="24" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="13">
-        <v>44538</v>
+      <c r="B24" s="38">
+        <v>44516</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24"/>
+        <v>12</v>
+      </c>
+      <c r="D24" s="29"/>
       <c r="E24" s="9">
-        <v>20</v>
-      </c>
-      <c r="F24" s="11">
+        <v>-10</v>
+      </c>
+      <c r="F24" s="10">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
     </row>
     <row r="25" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="13">
-        <v>44545</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25"/>
+      <c r="B25" s="42">
+        <v>44518</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="29"/>
       <c r="E25" s="9">
         <v>20</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
     </row>
     <row r="26" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="13">
-        <v>44547</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26"/>
-      <c r="E26" s="9">
+      <c r="B26" s="42">
+        <v>44525</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="41">
         <v>10</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="10">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I26" s="5"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
     </row>
     <row r="27" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="13">
-        <v>44551</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27"/>
+      <c r="B27" s="38">
+        <v>44526</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="29"/>
       <c r="E27" s="9">
         <v>20</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="10">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H27" s="6"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
     </row>
     <row r="28" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="13">
-        <v>44562</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28"/>
-      <c r="E28" s="12">
-        <v>10</v>
-      </c>
-      <c r="F28" s="11">
+      <c r="B28" s="38">
+        <v>44529</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="9">
+        <v>-10</v>
+      </c>
+      <c r="F28" s="10">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H28" s="7"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
     </row>
     <row r="29" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="31"/>
-      <c r="C29" s="30"/>
+      <c r="B29" s="38">
+        <v>44538</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>17</v>
+      </c>
       <c r="D29" s="29"/>
+      <c r="E29" s="9">
+        <v>20</v>
+      </c>
       <c r="F29" s="11">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="G29" s="7"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
     </row>
     <row r="30" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="B30" s="38">
+        <v>44545</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="9">
+        <v>20</v>
+      </c>
+      <c r="F30" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="B31" s="38">
+        <v>44547</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="9">
+        <v>10</v>
+      </c>
+      <c r="F31" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="38">
+        <v>44551</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="29"/>
+      <c r="E32" s="9">
+        <v>20</v>
+      </c>
+      <c r="F32" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="38">
+        <v>44562</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="12">
+        <v>10</v>
+      </c>
+      <c r="F33" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="31"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="29"/>
+      <c r="F34" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="H17:L20"/>
+    <mergeCell ref="H17:L24"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="B2:L14"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline with Milestones in this worksheet. Enter details in Project Details table. Chart is in cell B2 and Tip is in cell H17" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Line chart showing each milestone on the corresponding timeframe is in cell below" sqref="B1:C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter project details in table below" sqref="B15"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="B16"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Milestone in this column under this heading" sqref="C16"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Assigned To name in this column under this heading" sqref="D16"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter chart Position in this column under this heading. Project Timeline Tip is in cell at right" sqref="E16"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project Timeline Tip is in cell below" sqref="H16:I16"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline with Milestones in this worksheet. Enter details in Project Details table. Chart is in cell B2 and Tip is in cell H17" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Line chart showing each milestone on the corresponding timeframe is in cell below" sqref="B1:C1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter project details in table below" sqref="B15" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="B16" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Milestone in this column under this heading" sqref="C16" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Assigned To name in this column under this heading" sqref="D16" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter chart Position in this column under this heading. Project Timeline Tip is in cell at right" sqref="E16" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project Timeline Tip is in cell below" sqref="H16:I16" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3218,20 +3613,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3254,6 +3649,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9EFE20-B0BF-4817-AA37-C0305E12107B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71E3CE6-3BAB-4EFC-B954-0CB76BF2E2C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3261,12 +3664,4 @@
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9EFE20-B0BF-4817-AA37-C0305E12107B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>